<commit_message>
Template Datos Efecto Hall
</commit_message>
<xml_diff>
--- a/4. Efecto Hall/CompleteData/Datos_Todo.xlsx
+++ b/4. Efecto Hall/CompleteData/Datos_Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\Intermedio\4. Efecto Hall\CompleteData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF842D4C-C537-42A8-9C69-77187F0BD5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE20CF1-BFB1-45B5-AC06-464DA9D2856E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{B773243A-9F3D-47AF-B5C0-52D66A9AC8B3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B773243A-9F3D-47AF-B5C0-52D66A9AC8B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Caracterización" sheetId="1" r:id="rId1"/>
@@ -2521,7 +2521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF40345C-79AA-4416-B42D-9F09D94C5310}">
   <dimension ref="D2:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -4442,8 +4442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2412CE-1271-4303-B27D-2D9F18ABBAF1}">
   <dimension ref="A2:H77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>